<commit_message>
revision of the order of class attributes
</commit_message>
<xml_diff>
--- a/openpy_fx_tools_dss/Examples/37Bus/xlsx_files/BBDD_DSS_37BusIEEE.xlsx
+++ b/openpy_fx_tools_dss/Examples/37Bus/xlsx_files/BBDD_DSS_37BusIEEE.xlsx
@@ -59,6 +59,7 @@
     <sheet name="Sensor" sheetId="50" state="visible" r:id="rId50"/>
     <sheet name="FMonitor" sheetId="51" state="visible" r:id="rId51"/>
     <sheet name="Generic5" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="Switch" sheetId="53" state="visible" r:id="rId53"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15042,6 +15043,222 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Id_Switch</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>linecode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmatrix</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>xmatrix</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>cmatrix</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rg</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Xg</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rho</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>geometry</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>spacing</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wires</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EarthModel</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cncables</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tscables</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>B0</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Seasons</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Ratings</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>LineType</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>normamps</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>emergamps</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>faultrate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pctperm</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>repair</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>basefreq</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>enabled</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>like</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>